<commit_message>
feat(pivot-tables): add employee and salary aggregations
- Built PivotTables to analyze:
  - Employee counts by Job Title, Home Owner status, and Region
  - Salary sums by Education Level and Region
  - Bike Purchase rates by Region (Y/N percentages)
  - Avg Bike Satisfaction by Marital Status
- Included key metrics:
  - Highest employee counts: Director (21), Home Owners (51), Americas (24)
  - Highest salary sums: PhD ($1.83M), Americas ($2.10M)
  - Regional bike purchase trends (Asia 52% N, Europe 63% N)
</commit_message>
<xml_diff>
--- a/questions_and_analysis/employee_dataset.xlsx
+++ b/questions_and_analysis/employee_dataset.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="8327" windowHeight="9203" activeTab="4"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="8327" windowHeight="9203" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="employee_dataset" sheetId="1" r:id="rId1"/>
@@ -17,17 +17,21 @@
     <sheet name="employee_dataset_copy" sheetId="3" r:id="rId3"/>
     <sheet name="clean_dataset" sheetId="4" r:id="rId4"/>
     <sheet name="Logic&amp;C.Formatting" sheetId="5" r:id="rId5"/>
+    <sheet name="Pivot_Tables" sheetId="6" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">employee_dataset_copy!$A$1:$Z$86</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Logic&amp;C.Formatting'!$E$1:$R$86</definedName>
   </definedNames>
   <calcPr calcId="162913"/>
+  <pivotCaches>
+    <pivotCache cacheId="27" r:id="rId7"/>
+  </pivotCaches>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4990" uniqueCount="588">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5071" uniqueCount="614">
   <si>
     <t>Employee ID</t>
   </si>
@@ -2213,11 +2217,226 @@
         IF(H2="Salesman", "Raise dependent on Sales", "")</t>
     </r>
   </si>
+  <si>
+    <t>3. Summaries &amp; Aggregations with PivotTables</t>
+  </si>
+  <si>
+    <t>Q1: Count total employees per Region, per Job Title, per Home Owner status.</t>
+  </si>
+  <si>
+    <t>Q2: Sum of Salary by Region / Education Level.</t>
+  </si>
+  <si>
+    <t>Q3: Compare Bike Purchase (Y/N) rates across Region.</t>
+  </si>
+  <si>
+    <t>Q4: Average Bike Satisfaction by Marital Status.</t>
+  </si>
+  <si>
+    <t>Row Labels</t>
+  </si>
+  <si>
+    <t>Grand Total</t>
+  </si>
+  <si>
+    <t>Count of Employee ID</t>
+  </si>
+  <si>
+    <t>Column Labels</t>
+  </si>
+  <si>
+    <t>Count by Job Title</t>
+  </si>
+  <si>
+    <t>Count by Home Status</t>
+  </si>
+  <si>
+    <t>Count by Region</t>
+  </si>
+  <si>
+    <t>Sum of Salary</t>
+  </si>
+  <si>
+    <t>Salary Sum by Education Level</t>
+  </si>
+  <si>
+    <t>Salary Sum by Region</t>
+  </si>
+  <si>
+    <t>Count of Bike Purchase</t>
+  </si>
+  <si>
+    <t>Average of Bike Satisfaction</t>
+  </si>
+  <si>
+    <t>Bike Purchase (Y/N) rates across Region.</t>
+  </si>
+  <si>
+    <t>Average Bike Satisfaction by Marital Status.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Answer: by Region:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Africa 11, Americas 24, Asia 21, Europe 16, Pacific 13
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Answer:  by Home Status:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> N 34, Y 51</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Answer: by Job Title:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Accountant 4, Analyst 12, Clerical 8, Director 21, Engineer 6, HR 10, Manager 4, Professional 3, Receptionist 3, Salesman 8, Skilled Manual 6
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Answer: by Education Level:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Bachelors  $1,674,000.00 , High School  $1,390,000.00 , Masters  $1,472,000.00 , Partial College  $1,549,000.00 , PhD  $1,833,000.00 
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Answer: by Region:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Africa  $1,060,000.00 , Americas  $2,103,000.00 , Asia  $2,087,000.00 , Europe  $1,351,000.00 , Pacific  $1,317,000.00 
+  </t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Answer: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Africa 54.55% 45.45%, Americas 66.67% 33.33%, Asia 47.62% 52.38%, Europe 37.50% 62.50%, Pacific 61.54% 38.46%</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">
+</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t>Answer:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Century Gothic"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Divorced 2.13, Married 2.31, Single 2.24, Widowed 2.00</t>
+    </r>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="22" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -2382,7 +2601,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="33">
+  <fills count="34">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2562,6 +2781,12 @@
         <bgColor indexed="65"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.39997558519241921"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="10">
     <border>
@@ -2724,7 +2949,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -2759,6 +2984,21 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" pivotButton="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
   </cellXfs>
@@ -2807,43 +3047,9 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="27">
+  <dxfs count="7">
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <fill>
@@ -2873,192 +3079,13 @@
       </fill>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
     <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF00B050"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="9" tint="0.59996337778862885"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF00B050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <fgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FF9C0006"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFFC7CE"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="34" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -3114,6 +3141,2356 @@
     <xdr:clientData/>
   </xdr:twoCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1" refreshedBy="Dumisani Maxwell Mukuchura" refreshedDate="45771.943088657405" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="85">
+  <cacheSource type="worksheet">
+    <worksheetSource ref="A1:R86" sheet="clean_dataset"/>
+  </cacheSource>
+  <cacheFields count="18">
+    <cacheField name="Employee ID" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="1001" maxValue="1085"/>
+    </cacheField>
+    <cacheField name="First Name" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Last Name" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Personal Email" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Age" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="21" maxValue="65"/>
+    </cacheField>
+    <cacheField name="Gender" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Marital Status" numFmtId="0">
+      <sharedItems count="4">
+        <s v="Married"/>
+        <s v="Widowed"/>
+        <s v="Divorced"/>
+        <s v="Single"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Job Title" numFmtId="0">
+      <sharedItems count="11">
+        <s v="HR"/>
+        <s v="Analyst"/>
+        <s v="Manager"/>
+        <s v="Engineer"/>
+        <s v="Professional"/>
+        <s v="Salesman"/>
+        <s v="Director"/>
+        <s v="Clerical"/>
+        <s v="Receptionist"/>
+        <s v="Skilled Manual"/>
+        <s v="Accountant"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Salary" numFmtId="0">
+      <sharedItems containsSemiMixedTypes="0" containsString="0" containsNumber="1" containsInteger="1" minValue="30000" maxValue="148000"/>
+    </cacheField>
+    <cacheField name="Education Level" numFmtId="0">
+      <sharedItems count="5">
+        <s v="PhD"/>
+        <s v="High School"/>
+        <s v="Bachelors"/>
+        <s v="Masters"/>
+        <s v="Partial College"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Home Owner" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Y"/>
+        <s v="N"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Car Owner" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Commute Distance" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Start Date" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="End Date fixed" numFmtId="0">
+      <sharedItems/>
+    </cacheField>
+    <cacheField name="Region" numFmtId="0">
+      <sharedItems count="5">
+        <s v="Pacific"/>
+        <s v="Europe"/>
+        <s v="Asia"/>
+        <s v="Americas"/>
+        <s v="Africa"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Bike Purchase" numFmtId="0">
+      <sharedItems count="2">
+        <s v="Y"/>
+        <s v="N"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="Bike Satisfaction" numFmtId="0">
+      <sharedItems containsMixedTypes="1" containsNumber="1" containsInteger="1" minValue="0" maxValue="5"/>
+    </cacheField>
+  </cacheFields>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheRecords1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheRecords xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" count="85">
+  <r>
+    <n v="1084"/>
+    <s v="Pat"/>
+    <s v="Smith"/>
+    <s v="pat.smith@gmail.com"/>
+    <n v="61"/>
+    <s v="Male"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="85000"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="02/26/2010"/>
+    <s v="12/08/2017"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="1031"/>
+    <s v="Chris"/>
+    <s v="Williams"/>
+    <s v="chris.williams@live.com"/>
+    <n v="42"/>
+    <s v="Male"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="87000"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="01/18/2000"/>
+    <s v="09/23/2015"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <n v="1057"/>
+    <s v="Chris"/>
+    <s v="Williams"/>
+    <s v="chris.williams@hotmail.com"/>
+    <n v="50"/>
+    <s v="Male"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="145000"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="0-1 Miles"/>
+    <s v="05/26/2002"/>
+    <s v="03/01/2006"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="1025"/>
+    <s v="Jordan"/>
+    <s v="Wilson"/>
+    <s v="jordan.wilson@company.com"/>
+    <n v="49"/>
+    <s v="Female"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="60000"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="2-5 Miles"/>
+    <s v="01/07/2019"/>
+    <s v="01/24/2023"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1017"/>
+    <s v="John"/>
+    <s v="Brown"/>
+    <s v="john.brown@outlook.com"/>
+    <n v="27"/>
+    <s v="Female"/>
+    <x v="1"/>
+    <x v="4"/>
+    <n v="147000"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="1-2 Miles"/>
+    <s v="07/03/2003"/>
+    <s v="01/11/2023"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="1024"/>
+    <s v="Jane"/>
+    <s v="Williams"/>
+    <s v="jane.williams@gmail.com"/>
+    <n v="48"/>
+    <s v="Male"/>
+    <x v="1"/>
+    <x v="5"/>
+    <n v="134000"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="2-5 Miles"/>
+    <s v="01/08/2011"/>
+    <s v="11/30/2013"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1003"/>
+    <s v="Alex"/>
+    <s v="Brown"/>
+    <s v="alex.brown@gmail.com"/>
+    <n v="45"/>
+    <s v="Male"/>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="72000"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="Over 10 Miles"/>
+    <s v="03/20/2015"/>
+    <s v="Present"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="1028"/>
+    <s v="Taylor"/>
+    <s v="Davis"/>
+    <s v="taylor.davis@company.com"/>
+    <n v="63"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="46000"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="05/19/2020"/>
+    <s v="05/04/2022"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="1029"/>
+    <s v="Jordan"/>
+    <s v="Brown"/>
+    <s v="jordan.brown@outlook.com"/>
+    <n v="41"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="56000"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="2-5 Miles"/>
+    <s v="01/05/2010"/>
+    <s v="06/27/2021"/>
+    <x v="4"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1014"/>
+    <s v="Alex"/>
+    <s v="Miller"/>
+    <s v="alex.miller@company.com"/>
+    <n v="59"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="66000"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="5-10 Miles"/>
+    <s v="03/15/2015"/>
+    <s v=""/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="1064"/>
+    <s v="Jordan"/>
+    <s v="Jones"/>
+    <s v="jordan.jones@live.com"/>
+    <n v="33"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="7"/>
+    <n v="128000"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="Over 10 Miles"/>
+    <s v="07/14/2015"/>
+    <s v="08/30/2015"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1070"/>
+    <s v="Morgan"/>
+    <s v="Johnson"/>
+    <s v="morgan.johnson@live.com"/>
+    <n v="30"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="7"/>
+    <n v="112000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="5-10 Miles"/>
+    <s v="01/15/2011"/>
+    <s v="Present"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1077"/>
+    <s v="Morgan"/>
+    <s v="Miller"/>
+    <s v="morgan.miller@outlook.com"/>
+    <n v="49"/>
+    <s v="Female"/>
+    <x v="2"/>
+    <x v="8"/>
+    <n v="41000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="2-5 Miles"/>
+    <s v="01/23/2015"/>
+    <s v="06/19/2021"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="1015"/>
+    <s v="Taylor"/>
+    <s v="Smith"/>
+    <s v="taylor.smith@gmail.com"/>
+    <n v="37"/>
+    <s v="Male"/>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="96000"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="1-2 Miles"/>
+    <s v="11/06/2003"/>
+    <s v="01/03/2014"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1001"/>
+    <s v="Casey"/>
+    <s v="Anderson"/>
+    <s v="casey.anderson@hotmail.com"/>
+    <n v="64"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="66000"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="2-5 Miles"/>
+    <s v="04/19/2014"/>
+    <s v="08/16/2019"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="1022"/>
+    <s v="Morgan"/>
+    <s v="Taylor"/>
+    <s v="morgan.taylor@company.com"/>
+    <n v="51"/>
+    <s v="Male"/>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="105000"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="07/15/2003"/>
+    <s v="03/16/2018"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="1004"/>
+    <s v="Jane"/>
+    <s v="Brown"/>
+    <s v="jane.brown@outlook.com"/>
+    <n v="41"/>
+    <s v="Male"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="121000"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="2-5 Miles"/>
+    <s v="01/28/2017"/>
+    <s v="01/26/2020"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="1030"/>
+    <s v="Jordan"/>
+    <s v="Taylor"/>
+    <s v="jordan.taylor@company.com"/>
+    <n v="48"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="7"/>
+    <n v="60000"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="5-10 Miles"/>
+    <s v="06/29/2007"/>
+    <s v="12/13/2016"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="1062"/>
+    <s v="Jordan"/>
+    <s v="Brown"/>
+    <s v="jordan.brown@gmail.com"/>
+    <n v="53"/>
+    <s v="Female"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="47000"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="2-5 Miles"/>
+    <s v="01/02/2000"/>
+    <s v="01/10/2002"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="1080"/>
+    <s v="Chris"/>
+    <s v="Miller"/>
+    <s v="chris.miller@gmail.com"/>
+    <n v="44"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="54000"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="09/09/2018"/>
+    <s v="12/17/2020"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1036"/>
+    <s v="Jane"/>
+    <s v="Jones"/>
+    <s v="jane.jones@company.com"/>
+    <n v="55"/>
+    <s v="Female"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="96000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="5-10 Miles"/>
+    <s v="01/08/2011"/>
+    <s v="02/08/2018"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="1012"/>
+    <s v="Alex"/>
+    <s v="Smith"/>
+    <s v="alex.smith@gmail.com"/>
+    <n v="37"/>
+    <s v="Male"/>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="142000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="Over 10 Miles"/>
+    <s v="10/09/2016"/>
+    <s v="02/20/2021"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1085"/>
+    <s v="Morgan"/>
+    <s v="Miller"/>
+    <s v="morgan.miller@outlook.com"/>
+    <n v="65"/>
+    <s v="Female"/>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="91000"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="5-10 Miles"/>
+    <s v="03/28/2003"/>
+    <s v="08/15/2008"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <n v="1045"/>
+    <s v="Casey"/>
+    <s v="Williams"/>
+    <s v="casey.williams@live.com"/>
+    <n v="43"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="115000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="04/21/2000"/>
+    <s v="06/04/2006"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1074"/>
+    <s v="Jordan"/>
+    <s v="Smith"/>
+    <s v="jordan.smith@gmail.com"/>
+    <n v="23"/>
+    <s v="Female"/>
+    <x v="2"/>
+    <x v="5"/>
+    <n v="66000"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="04/15/2004"/>
+    <s v="12/11/2008"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <n v="1006"/>
+    <s v="Morgan"/>
+    <s v="Wilson"/>
+    <s v="morgan.wilson@company.com"/>
+    <n v="47"/>
+    <s v="Male"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="36000"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="2-5 Miles"/>
+    <s v="01/09/2007"/>
+    <s v="01/01/2022"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1026"/>
+    <s v="Jane"/>
+    <s v="Taylor"/>
+    <s v="jane.taylor@gmail.com"/>
+    <n v="63"/>
+    <s v="Female"/>
+    <x v="0"/>
+    <x v="3"/>
+    <n v="73000"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="1-2 Miles"/>
+    <s v="05/30/2011"/>
+    <s v="01/25/2016"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="1078"/>
+    <s v="Pat"/>
+    <s v="Jones"/>
+    <s v="pat.jones@hotmail.com"/>
+    <n v="41"/>
+    <s v="Male"/>
+    <x v="1"/>
+    <x v="9"/>
+    <n v="146000"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="1-2 Miles"/>
+    <s v="01/07/2012"/>
+    <s v="02/20/2017"/>
+    <x v="4"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="1075"/>
+    <s v="Taylor"/>
+    <s v="Taylor"/>
+    <s v="taylor.taylor@live.com"/>
+    <n v="28"/>
+    <s v="Female"/>
+    <x v="0"/>
+    <x v="5"/>
+    <n v="131000"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="08/01/2018"/>
+    <s v="Present"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="1063"/>
+    <s v="Pat"/>
+    <s v="Williams"/>
+    <s v="pat.williams@outlook.com"/>
+    <n v="31"/>
+    <s v="Female"/>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="121000"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="2-5 Miles"/>
+    <s v="01/19/2018"/>
+    <s v="03/31/2020"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="1"/>
+  </r>
+  <r>
+    <n v="1066"/>
+    <s v="Jordan"/>
+    <s v="Wilson"/>
+    <s v="jordan.wilson@company.com"/>
+    <n v="55"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="10"/>
+    <n v="111000"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="1-2 Miles"/>
+    <s v="01/10/2005"/>
+    <s v=""/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1002"/>
+    <s v="Casey"/>
+    <s v="Williams"/>
+    <s v="casey.williams@outlook.com"/>
+    <n v="38"/>
+    <s v="Male"/>
+    <x v="0"/>
+    <x v="10"/>
+    <n v="111000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="09/16/2004"/>
+    <s v="01/26/2020"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="1019"/>
+    <s v="Jane"/>
+    <s v="Smith"/>
+    <s v="jane.smith@hotmail.com"/>
+    <n v="31"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="5"/>
+    <n v="83000"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="01/24/2007"/>
+    <s v="11/04/2010"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <n v="1049"/>
+    <s v="Jamie"/>
+    <s v="Brown"/>
+    <s v="jamie.brown@hotmail.com"/>
+    <n v="58"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="2"/>
+    <n v="46000"/>
+    <x v="4"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="07/17/2005"/>
+    <s v="01/02/2023"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="1037"/>
+    <s v="John"/>
+    <s v="Smith"/>
+    <s v="john.smith@outlook.com"/>
+    <n v="31"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="134000"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="03/01/2008"/>
+    <s v="01/04/2019"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1079"/>
+    <s v="Pat"/>
+    <s v="Taylor"/>
+    <s v="pat.taylor@hotmail.com"/>
+    <n v="58"/>
+    <s v="Male"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="46000"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="01/23/2019"/>
+    <s v="09/03/2021"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1007"/>
+    <s v="Jamie"/>
+    <s v="Miller"/>
+    <s v="jamie.miller@hotmail.com"/>
+    <n v="46"/>
+    <s v="Male"/>
+    <x v="1"/>
+    <x v="9"/>
+    <n v="94000"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="0-1 Miles"/>
+    <s v="03/31/2008"/>
+    <s v="11/11/2008"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1059"/>
+    <s v="Taylor"/>
+    <s v="Davis"/>
+    <s v="taylor.davis@live.com"/>
+    <n v="22"/>
+    <s v="Female"/>
+    <x v="2"/>
+    <x v="8"/>
+    <n v="79000"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="5-10 Miles"/>
+    <s v="01/24/2016"/>
+    <s v="01/24/2021"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1011"/>
+    <s v="Pat"/>
+    <s v="Smith"/>
+    <s v="pat.smith@company.com"/>
+    <n v="64"/>
+    <s v="Female"/>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="57000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="01/16/2018"/>
+    <s v="12/15/2023"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1013"/>
+    <s v="Jamie"/>
+    <s v="Brown"/>
+    <s v="jamie.brown@live.com"/>
+    <n v="35"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="4"/>
+    <n v="80000"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="08/22/2004"/>
+    <s v="09/06/2023"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="1054"/>
+    <s v="John"/>
+    <s v="Johnson"/>
+    <s v="john.johnson@outlook.com"/>
+    <n v="27"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="9"/>
+    <n v="142000"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="0-1 Miles"/>
+    <s v="10/29/2005"/>
+    <s v="01/15/2019"/>
+    <x v="4"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1055"/>
+    <s v="Morgan"/>
+    <s v="Williams"/>
+    <s v="morgan.williams@outlook.com"/>
+    <n v="33"/>
+    <s v="Female"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="89000"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="Over 10 Miles"/>
+    <s v="06/06/2007"/>
+    <s v="12/06/2011"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1068"/>
+    <s v="Chris"/>
+    <s v="Miller"/>
+    <s v="chris.miller@outlook.com"/>
+    <n v="55"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="83000"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="2-5 Miles"/>
+    <s v="05/23/2014"/>
+    <s v="Present"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1033"/>
+    <s v="Chris"/>
+    <s v="Johnson"/>
+    <s v="chris.johnson@company.com"/>
+    <n v="48"/>
+    <s v="Female"/>
+    <x v="0"/>
+    <x v="7"/>
+    <n v="75000"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="12/20/2016"/>
+    <s v="01/15/2021"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1020"/>
+    <s v="Jamie"/>
+    <s v="Wilson"/>
+    <s v="jamie.wilson@live.com"/>
+    <n v="53"/>
+    <s v="Male"/>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="34000"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="12/23/2007"/>
+    <s v="09/07/2020"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="1027"/>
+    <s v="Morgan"/>
+    <s v="Brown"/>
+    <s v="morgan.brown@gmail.com"/>
+    <n v="57"/>
+    <s v="Female"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="115000"/>
+    <x v="4"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="2-5 Miles"/>
+    <s v="03/13/2000"/>
+    <s v="10/11/2016"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1061"/>
+    <s v="Jordan"/>
+    <s v="Wilson"/>
+    <s v="jordan.wilson@hotmail.com"/>
+    <n v="45"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="7"/>
+    <n v="117000"/>
+    <x v="4"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="2-5 Miles"/>
+    <s v="09/08/2014"/>
+    <s v="12/29/2014"/>
+    <x v="4"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1056"/>
+    <s v="Taylor"/>
+    <s v="Wilson"/>
+    <s v="taylor.wilson@gmail.com"/>
+    <n v="55"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="7"/>
+    <n v="117000"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="05/02/2002"/>
+    <s v="01/13/2018"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <n v="1010"/>
+    <s v="Pat"/>
+    <s v="Williams"/>
+    <s v="pat.williams@company.com"/>
+    <n v="52"/>
+    <s v="Female"/>
+    <x v="1"/>
+    <x v="7"/>
+    <n v="66000"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="5-10 Miles"/>
+    <s v="02/13/2004"/>
+    <s v="06/21/2013"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1018"/>
+    <s v="Jamie"/>
+    <s v="Taylor"/>
+    <s v="jamie.taylor@company.com"/>
+    <n v="42"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="5"/>
+    <n v="39000"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="1-2 Miles"/>
+    <s v="05/08/2010"/>
+    <s v="06/10/2021"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <n v="1060"/>
+    <s v="Casey"/>
+    <s v="Taylor"/>
+    <s v="casey.taylor@company.com"/>
+    <n v="45"/>
+    <s v="Female"/>
+    <x v="1"/>
+    <x v="2"/>
+    <n v="142000"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="2-5 Miles"/>
+    <s v="05/28/2006"/>
+    <s v="06/09/2021"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1058"/>
+    <s v="Casey"/>
+    <s v="Smith"/>
+    <s v="casey.smith@hotmail.com"/>
+    <n v="55"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="5"/>
+    <n v="87000"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="2-5 Miles"/>
+    <s v="07/14/2017"/>
+    <s v="04/02/2022"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="1042"/>
+    <s v="Alex"/>
+    <s v="Miller"/>
+    <s v="alex.miller@gmail.com"/>
+    <n v="21"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="123000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="2-5 Miles"/>
+    <s v="01/04/2020"/>
+    <s v="02/02/2022"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="5"/>
+  </r>
+  <r>
+    <n v="1065"/>
+    <s v="Chris"/>
+    <s v="Williams"/>
+    <s v="chris.williams@company.com"/>
+    <n v="56"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="108000"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="12/20/2003"/>
+    <s v="01/19/2006"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="1046"/>
+    <s v="Jordan"/>
+    <s v="Taylor"/>
+    <s v="jordan.taylor@live.com"/>
+    <n v="58"/>
+    <s v="Female"/>
+    <x v="1"/>
+    <x v="10"/>
+    <n v="70000"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="Over 10 Miles"/>
+    <s v="10/03/2016"/>
+    <s v="01/23/2021"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1009"/>
+    <s v="Jordan"/>
+    <s v="Williams"/>
+    <s v="jordan.williams@outlook.com"/>
+    <n v="29"/>
+    <s v="Male"/>
+    <x v="1"/>
+    <x v="8"/>
+    <n v="81000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="5-10 Miles"/>
+    <s v="01/26/2017"/>
+    <s v="01/08/2023"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="1072"/>
+    <s v="Jordan"/>
+    <s v="Williams"/>
+    <s v="jordan.williams@outlook.com"/>
+    <n v="27"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="80000"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="11/11/2014"/>
+    <s v="09/17/2017"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1081"/>
+    <s v="John"/>
+    <s v="Jones"/>
+    <s v="john.jones@outlook.com"/>
+    <n v="27"/>
+    <s v="Female"/>
+    <x v="1"/>
+    <x v="9"/>
+    <n v="120000"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="2-5 Miles"/>
+    <s v="09/13/2017"/>
+    <s v="01/05/2023"/>
+    <x v="4"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1067"/>
+    <s v="Taylor"/>
+    <s v="Smith"/>
+    <s v="taylor.smith@gmail.com"/>
+    <n v="60"/>
+    <s v="Female"/>
+    <x v="0"/>
+    <x v="6"/>
+    <n v="130000"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="0-1 Miles"/>
+    <s v="01/20/2019"/>
+    <s v="01/25/2020"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1051"/>
+    <s v="Jamie"/>
+    <s v="Williams"/>
+    <s v="jamie.williams@hotmail.com"/>
+    <n v="23"/>
+    <s v="Male"/>
+    <x v="1"/>
+    <x v="10"/>
+    <n v="73000"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="1-2 Miles"/>
+    <s v="01/20/2000"/>
+    <s v="01/09/2015"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="1053"/>
+    <s v="Jane"/>
+    <s v="Anderson"/>
+    <s v="jane.anderson@hotmail.com"/>
+    <n v="27"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="5"/>
+    <n v="146000"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="07/29/2014"/>
+    <s v="11/27/2020"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1041"/>
+    <s v="Alex"/>
+    <s v="Miller"/>
+    <s v="alex.miller@hotmail.com"/>
+    <n v="37"/>
+    <s v="Female"/>
+    <x v="1"/>
+    <x v="3"/>
+    <n v="51000"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="06/07/2019"/>
+    <s v="01/04/2020"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1071"/>
+    <s v="Jordan"/>
+    <s v="Anderson"/>
+    <s v="jordan.anderson@company.com"/>
+    <n v="65"/>
+    <s v="Male"/>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="56000"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="Over 10 Miles"/>
+    <s v="09/02/2004"/>
+    <s v="12/18/2004"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1047"/>
+    <s v="Jamie"/>
+    <s v="Johnson"/>
+    <s v="jamie.johnson@gmail.com"/>
+    <n v="49"/>
+    <s v="Female"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="68000"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="Over 10 Miles"/>
+    <s v="08/19/2002"/>
+    <s v="06/21/2010"/>
+    <x v="4"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1069"/>
+    <s v="Morgan"/>
+    <s v="Johnson"/>
+    <s v="morgan.johnson@hotmail.com"/>
+    <n v="24"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="9"/>
+    <n v="126000"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="04/08/2005"/>
+    <s v="01/25/2016"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1082"/>
+    <s v="Alex"/>
+    <s v="Davis"/>
+    <s v="alex.davis@company.com"/>
+    <n v="64"/>
+    <s v="Female"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="116000"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="2-5 Miles"/>
+    <s v="03/15/2002"/>
+    <s v="04/06/2018"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="1034"/>
+    <s v="John"/>
+    <s v="Johnson"/>
+    <s v="john.johnson@gmail.com"/>
+    <n v="60"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="135000"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="01/02/2006"/>
+    <s v="05/25/2011"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1039"/>
+    <s v="Pat"/>
+    <s v="Williams"/>
+    <s v="pat.williams@hotmail.com"/>
+    <n v="24"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="144000"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="Over 10 Miles"/>
+    <s v="01/18/2017"/>
+    <s v="11/08/2018"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1052"/>
+    <s v="Alex"/>
+    <s v="Taylor"/>
+    <s v="alex.taylor@hotmail.com"/>
+    <n v="65"/>
+    <s v="Female"/>
+    <x v="1"/>
+    <x v="6"/>
+    <n v="65000"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="N"/>
+    <s v="5-10 Miles"/>
+    <s v="01/30/2017"/>
+    <s v=""/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="1043"/>
+    <s v="Alex"/>
+    <s v="Wilson"/>
+    <s v="alex.wilson@gmail.com"/>
+    <n v="63"/>
+    <s v="Female"/>
+    <x v="0"/>
+    <x v="1"/>
+    <n v="106000"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="2-5 Miles"/>
+    <s v="02/21/2001"/>
+    <s v="Present"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1005"/>
+    <s v="Taylor"/>
+    <s v="Miller"/>
+    <s v="taylor.miller@live.com"/>
+    <n v="25"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="89000"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="2-5 Miles"/>
+    <s v="10/24/2003"/>
+    <s v="08/07/2010"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1040"/>
+    <s v="Pat"/>
+    <s v="Taylor"/>
+    <s v="pat.taylor@company.com"/>
+    <n v="61"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="3"/>
+    <n v="91000"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="1-2 Miles"/>
+    <s v="04/13/2006"/>
+    <s v="01/31/2019"/>
+    <x v="0"/>
+    <x v="0"/>
+    <n v="2"/>
+  </r>
+  <r>
+    <n v="1038"/>
+    <s v="Chris"/>
+    <s v="Taylor"/>
+    <s v="chris.taylor@live.com"/>
+    <n v="52"/>
+    <s v="Female"/>
+    <x v="2"/>
+    <x v="1"/>
+    <n v="118000"/>
+    <x v="3"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="0-1 Miles"/>
+    <s v="06/03/2017"/>
+    <s v="01/25/2021"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="1021"/>
+    <s v="Alex"/>
+    <s v="Brown"/>
+    <s v="alex.brown@gmail.com"/>
+    <n v="34"/>
+    <s v="Female"/>
+    <x v="0"/>
+    <x v="9"/>
+    <n v="148000"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="03/30/2012"/>
+    <s v="03/18/2022"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1032"/>
+    <s v="Casey"/>
+    <s v="Brown"/>
+    <s v="casey.brown@outlook.com"/>
+    <n v="25"/>
+    <s v="Female"/>
+    <x v="0"/>
+    <x v="2"/>
+    <n v="148000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="0-1 Miles"/>
+    <s v="04/05/2014"/>
+    <s v="03/29/2015"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="4"/>
+  </r>
+  <r>
+    <n v="1048"/>
+    <s v="Alex"/>
+    <s v="Wilson"/>
+    <s v="alex.wilson@gmail.com"/>
+    <n v="64"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="109000"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="06/29/2008"/>
+    <s v="01/20/2018"/>
+    <x v="3"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="1050"/>
+    <s v="John"/>
+    <s v="Miller"/>
+    <s v="john.miller@hotmail.com"/>
+    <n v="48"/>
+    <s v="Male"/>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="52000"/>
+    <x v="2"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="0-1 Miles"/>
+    <s v="02/09/2018"/>
+    <s v="01/23/2022"/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1035"/>
+    <s v="Alex"/>
+    <s v="Davis"/>
+    <s v="alex.davis@company.com"/>
+    <n v="61"/>
+    <s v="Female"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="139000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="07/18/2002"/>
+    <s v="05/31/2005"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1008"/>
+    <s v="Jordan"/>
+    <s v="Davis"/>
+    <s v="jordan.davis@live.com"/>
+    <n v="27"/>
+    <s v="Male"/>
+    <x v="1"/>
+    <x v="0"/>
+    <n v="106000"/>
+    <x v="4"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="1-2 Miles"/>
+    <s v="04/23/2020"/>
+    <s v="09/10/2023"/>
+    <x v="2"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1076"/>
+    <s v="Chris"/>
+    <s v="Jones"/>
+    <s v="chris.jones@company.com"/>
+    <n v="57"/>
+    <s v="Male"/>
+    <x v="2"/>
+    <x v="5"/>
+    <n v="128000"/>
+    <x v="1"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="1-2 Miles"/>
+    <s v="06/29/2012"/>
+    <s v="01/16/2014"/>
+    <x v="4"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1083"/>
+    <s v="Taylor"/>
+    <s v="Jones"/>
+    <s v="taylor.jones@outlook.com"/>
+    <n v="42"/>
+    <s v="Female"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="30000"/>
+    <x v="0"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="2-5 Miles"/>
+    <s v="11/19/2005"/>
+    <s v=""/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1044"/>
+    <s v="Pat"/>
+    <s v="Miller"/>
+    <s v="pat.miller@hotmail.com"/>
+    <n v="35"/>
+    <s v="Male"/>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="65000"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="2-5 Miles"/>
+    <s v="12/22/2015"/>
+    <s v=""/>
+    <x v="1"/>
+    <x v="1"/>
+    <s v="N/A"/>
+  </r>
+  <r>
+    <n v="1023"/>
+    <s v="Jamie"/>
+    <s v="Wilson"/>
+    <s v="jamie.wilson@outlook.com"/>
+    <n v="36"/>
+    <s v="Male"/>
+    <x v="2"/>
+    <x v="6"/>
+    <n v="95000"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="N"/>
+    <s v="1-2 Miles"/>
+    <s v="04/16/2016"/>
+    <s v="09/06/2016"/>
+    <x v="2"/>
+    <x v="0"/>
+    <n v="3"/>
+  </r>
+  <r>
+    <n v="1073"/>
+    <s v="Pat"/>
+    <s v="Williams"/>
+    <s v="pat.williams@hotmail.com"/>
+    <n v="27"/>
+    <s v="Female"/>
+    <x v="3"/>
+    <x v="6"/>
+    <n v="42000"/>
+    <x v="0"/>
+    <x v="0"/>
+    <s v="Y"/>
+    <s v="2-5 Miles"/>
+    <s v="01/29/2013"/>
+    <s v="08/05/2018"/>
+    <x v="3"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+  <r>
+    <n v="1016"/>
+    <s v="Pat"/>
+    <s v="Johnson"/>
+    <s v="pat.johnson@company.com"/>
+    <n v="22"/>
+    <s v="Male"/>
+    <x v="2"/>
+    <x v="3"/>
+    <n v="68000"/>
+    <x v="3"/>
+    <x v="1"/>
+    <s v="Y"/>
+    <s v="1-2 Miles"/>
+    <s v="06/17/2019"/>
+    <s v="03/30/2022"/>
+    <x v="1"/>
+    <x v="1"/>
+    <n v="0"/>
+  </r>
+</pivotCacheRecords>
+</file>
+
+<file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable7" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="H29:I34" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="18">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="5">
+        <item x="2"/>
+        <item x="0"/>
+        <item x="3"/>
+        <item x="1"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="6"/>
+  </rowFields>
+  <rowItems count="5">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Average of Bike Satisfaction" fld="17" subtotal="average" baseField="6" baseItem="0"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="0">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="6" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable6" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A29:D36" firstHeaderRow="1" firstDataRow="2" firstDataCol="1"/>
+  <pivotFields count="18">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField axis="axisCol" dataField="1" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="15"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colFields count="1">
+    <field x="16"/>
+  </colFields>
+  <colItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Bike Purchase" fld="16" subtotal="count" showDataAs="percentOfRow" baseField="15" baseItem="0" numFmtId="10"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable5" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E19:F25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="18">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="15"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Salary" fld="8" baseField="0" baseItem="0" numFmtId="44"/>
+  </dataFields>
+  <formats count="1">
+    <format dxfId="4">
+      <pivotArea outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable4" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A19:B25" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="18">
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="2"/>
+        <item x="1"/>
+        <item x="3"/>
+        <item x="4"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="9"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Sum of Salary" fld="8" baseField="0" baseItem="0"/>
+  </dataFields>
+  <formats count="2">
+    <format dxfId="6">
+      <pivotArea collapsedLevelsAreSubtotals="1" fieldPosition="0">
+        <references count="1">
+          <reference field="9" count="0"/>
+        </references>
+      </pivotArea>
+    </format>
+    <format dxfId="5">
+      <pivotArea grandRow="1" outline="0" collapsedLevelsAreSubtotals="1" fieldPosition="0"/>
+    </format>
+  </formats>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable3" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="I3:J9" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="18">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="6">
+        <item x="4"/>
+        <item x="3"/>
+        <item x="2"/>
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="15"/>
+  </rowFields>
+  <rowItems count="6">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Employee ID" fld="0" subtotal="count" baseField="15" baseItem="0"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable2" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="E3:F6" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="18">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="3">
+        <item x="1"/>
+        <item x="0"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="10"/>
+  </rowFields>
+  <rowItems count="3">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Employee ID" fld="0" subtotal="count" baseField="0" baseItem="1171936"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
+</file>
+
+<file path=xl/pivotTables/pivotTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="PivotTable1" cacheId="27" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0">
+  <location ref="A3:B15" firstHeaderRow="1" firstDataRow="1" firstDataCol="1"/>
+  <pivotFields count="18">
+    <pivotField dataField="1" showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField axis="axisRow" showAll="0">
+      <items count="12">
+        <item sd="0" x="10"/>
+        <item sd="0" x="1"/>
+        <item sd="0" x="7"/>
+        <item sd="0" x="6"/>
+        <item sd="0" x="3"/>
+        <item sd="0" x="0"/>
+        <item sd="0" x="2"/>
+        <item sd="0" x="4"/>
+        <item sd="0" x="8"/>
+        <item sd="0" x="5"/>
+        <item sd="0" x="9"/>
+        <item t="default"/>
+      </items>
+    </pivotField>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0"/>
+    <pivotField showAll="0" defaultSubtotal="0"/>
+  </pivotFields>
+  <rowFields count="1">
+    <field x="7"/>
+  </rowFields>
+  <rowItems count="12">
+    <i>
+      <x/>
+    </i>
+    <i>
+      <x v="1"/>
+    </i>
+    <i>
+      <x v="2"/>
+    </i>
+    <i>
+      <x v="3"/>
+    </i>
+    <i>
+      <x v="4"/>
+    </i>
+    <i>
+      <x v="5"/>
+    </i>
+    <i>
+      <x v="6"/>
+    </i>
+    <i>
+      <x v="7"/>
+    </i>
+    <i>
+      <x v="8"/>
+    </i>
+    <i>
+      <x v="9"/>
+    </i>
+    <i>
+      <x v="10"/>
+    </i>
+    <i t="grand">
+      <x/>
+    </i>
+  </rowItems>
+  <colItems count="1">
+    <i/>
+  </colItems>
+  <dataFields count="1">
+    <dataField name="Count of Employee ID" fld="0" subtotal="count" baseField="0" baseItem="1171936"/>
+  </dataFields>
+  <pivotTableStyleInfo name="PivotStyleLight16" showRowHeaders="1" showColHeaders="1" showRowStripes="0" showColStripes="0" showLastColumn="1"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{962EF5D1-5CA2-4c93-8EF4-DBF5C05439D2}">
+      <x14:pivotTableDefinition xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" hideValuesRow="1"/>
+    </ext>
+  </extLst>
+</pivotTableDefinition>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -8933,10 +11310,10 @@
   <sheetPr>
     <tabColor theme="4" tint="0.39997558519241921"/>
   </sheetPr>
-  <dimension ref="A1:U71"/>
+  <dimension ref="A1:U87"/>
   <sheetViews>
-    <sheetView topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="G77" sqref="G77"/>
+    <sheetView tabSelected="1" topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="G75" sqref="G75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.25"/>
@@ -9940,6 +12317,72 @@
     <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="5" t="s">
         <v>587</v>
+      </c>
+    </row>
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>589</v>
+      </c>
+    </row>
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A75" s="19" t="s">
+        <v>609</v>
+      </c>
+    </row>
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A76" s="5" t="s">
+        <v>608</v>
+      </c>
+    </row>
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A77" s="19" t="s">
+        <v>607</v>
+      </c>
+    </row>
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A78" s="19"/>
+    </row>
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>590</v>
+      </c>
+    </row>
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A80" s="19" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A81" s="19" t="s">
+        <v>611</v>
+      </c>
+    </row>
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A82" s="19"/>
+    </row>
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A83" s="28" t="s">
+        <v>591</v>
+      </c>
+    </row>
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A84" s="28" t="s">
+        <v>612</v>
+      </c>
+    </row>
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>592</v>
+      </c>
+    </row>
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A87" s="2" t="s">
+        <v>613</v>
       </c>
     </row>
   </sheetData>
@@ -17852,8 +20295,8 @@
   </sheetPr>
   <dimension ref="A1:R86"/>
   <sheetViews>
-    <sheetView topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="U19" sqref="U19"/>
+    <sheetView topLeftCell="G1" workbookViewId="0">
+      <selection activeCell="R2" sqref="R2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
@@ -17919,7 +20362,7 @@
         <v>12</v>
       </c>
       <c r="N1" s="4" t="s">
-        <v>349</v>
+        <v>13</v>
       </c>
       <c r="O1" s="4" t="s">
         <v>351</v>
@@ -17931,7 +20374,7 @@
         <v>16</v>
       </c>
       <c r="R1" s="4" t="s">
-        <v>354</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
@@ -22707,7 +25150,7 @@
   </sheetPr>
   <dimension ref="A1:AD87"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
+    <sheetView topLeftCell="U1" workbookViewId="0">
       <selection activeCell="AG24" sqref="AG24"/>
     </sheetView>
   </sheetViews>
@@ -28285,10 +30728,10 @@
   </sheetData>
   <autoFilter ref="E1:R86"/>
   <conditionalFormatting sqref="I1:I1048576">
-    <cfRule type="top10" dxfId="6" priority="8" rank="10"/>
+    <cfRule type="top10" dxfId="3" priority="8" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="E1:E1048576">
-    <cfRule type="top10" dxfId="5" priority="7" bottom="1" rank="10"/>
+    <cfRule type="top10" dxfId="2" priority="7" bottom="1" rank="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="R1:R1048576">
     <cfRule type="dataBar" priority="2">
@@ -28305,7 +30748,7 @@
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="N1:N1048576">
-    <cfRule type="expression" dxfId="4" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>YEAR(N2) &gt;= 2015</formula>
     </cfRule>
   </conditionalFormatting>
@@ -28330,4 +30773,482 @@
     </ext>
   </extLst>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor theme="9" tint="0.39997558519241921"/>
+  </sheetPr>
+  <dimension ref="A2:J36"/>
+  <sheetViews>
+    <sheetView topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="H30" sqref="H30:I33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.05" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="12.6640625" customWidth="1"/>
+    <col min="2" max="2" width="19.5546875" customWidth="1"/>
+    <col min="3" max="3" width="7" customWidth="1"/>
+    <col min="4" max="4" width="10.77734375" customWidth="1"/>
+    <col min="5" max="5" width="12.44140625" customWidth="1"/>
+    <col min="6" max="6" width="19.5546875" customWidth="1"/>
+    <col min="7" max="7" width="3.33203125" customWidth="1"/>
+    <col min="8" max="8" width="12.44140625" customWidth="1"/>
+    <col min="9" max="9" width="24.6640625" customWidth="1"/>
+    <col min="10" max="10" width="19.5546875" customWidth="1"/>
+    <col min="11" max="15" width="5.77734375" customWidth="1"/>
+    <col min="16" max="16" width="10.77734375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" s="23" t="s">
+        <v>597</v>
+      </c>
+      <c r="B2" s="24"/>
+      <c r="E2" s="23" t="s">
+        <v>598</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="I2" s="23" t="s">
+        <v>599</v>
+      </c>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="B3" t="s">
+        <v>595</v>
+      </c>
+      <c r="E3" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="F3" t="s">
+        <v>595</v>
+      </c>
+      <c r="I3" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="J3" t="s">
+        <v>595</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" s="21" t="s">
+        <v>403</v>
+      </c>
+      <c r="B4" s="22">
+        <v>4</v>
+      </c>
+      <c r="E4" s="21" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="22">
+        <v>34</v>
+      </c>
+      <c r="I4" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="22">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="B5" s="22">
+        <v>12</v>
+      </c>
+      <c r="E5" s="21" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="22">
+        <v>51</v>
+      </c>
+      <c r="I5" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="J5" s="22">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" s="21" t="s">
+        <v>87</v>
+      </c>
+      <c r="B6" s="22">
+        <v>8</v>
+      </c>
+      <c r="E6" s="21" t="s">
+        <v>594</v>
+      </c>
+      <c r="F6" s="22">
+        <v>85</v>
+      </c>
+      <c r="I6" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="J6" s="22">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="21" t="s">
+        <v>62</v>
+      </c>
+      <c r="B7" s="22">
+        <v>21</v>
+      </c>
+      <c r="I7" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="J7" s="22">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="21" t="s">
+        <v>83</v>
+      </c>
+      <c r="B8" s="22">
+        <v>6</v>
+      </c>
+      <c r="I8" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="J8" s="22">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" s="21" t="s">
+        <v>112</v>
+      </c>
+      <c r="B9" s="22">
+        <v>10</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>594</v>
+      </c>
+      <c r="J9" s="22">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" s="22">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" s="21" t="s">
+        <v>105</v>
+      </c>
+      <c r="B11" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="21" t="s">
+        <v>95</v>
+      </c>
+      <c r="B12" s="22">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" s="21" t="s">
+        <v>58</v>
+      </c>
+      <c r="B13" s="22">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" s="21" t="s">
+        <v>248</v>
+      </c>
+      <c r="B14" s="22">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" s="21" t="s">
+        <v>594</v>
+      </c>
+      <c r="B15" s="22">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A18" s="25" t="s">
+        <v>601</v>
+      </c>
+      <c r="B18" s="24"/>
+      <c r="E18" s="23" t="s">
+        <v>602</v>
+      </c>
+      <c r="F18" s="24"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A19" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="B19" t="s">
+        <v>600</v>
+      </c>
+      <c r="E19" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="F19" t="s">
+        <v>600</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A20" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="27">
+        <v>1674000</v>
+      </c>
+      <c r="E20" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="F20" s="27">
+        <v>1060000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A21" s="21" t="s">
+        <v>32</v>
+      </c>
+      <c r="B21" s="27">
+        <v>1390000</v>
+      </c>
+      <c r="E21" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="F21" s="27">
+        <v>2103000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A22" s="21" t="s">
+        <v>77</v>
+      </c>
+      <c r="B22" s="27">
+        <v>1472000</v>
+      </c>
+      <c r="E22" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="F22" s="27">
+        <v>2087000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A23" s="21" t="s">
+        <v>91</v>
+      </c>
+      <c r="B23" s="27">
+        <v>1549000</v>
+      </c>
+      <c r="E23" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="F23" s="27">
+        <v>1351000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A24" s="21" t="s">
+        <v>23</v>
+      </c>
+      <c r="B24" s="27">
+        <v>1833000</v>
+      </c>
+      <c r="E24" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="27">
+        <v>1317000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A25" s="21" t="s">
+        <v>594</v>
+      </c>
+      <c r="B25" s="27">
+        <v>7918000</v>
+      </c>
+      <c r="E25" s="21" t="s">
+        <v>594</v>
+      </c>
+      <c r="F25" s="27">
+        <v>7918000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A28" s="23" t="s">
+        <v>605</v>
+      </c>
+      <c r="B28" s="24"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="H28" s="23" t="s">
+        <v>606</v>
+      </c>
+      <c r="I28" s="23"/>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A29" s="20" t="s">
+        <v>603</v>
+      </c>
+      <c r="B29" s="20" t="s">
+        <v>596</v>
+      </c>
+      <c r="H29" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="I29" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A30" s="20" t="s">
+        <v>593</v>
+      </c>
+      <c r="B30" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" t="s">
+        <v>24</v>
+      </c>
+      <c r="D30" t="s">
+        <v>594</v>
+      </c>
+      <c r="H30" s="21" t="s">
+        <v>332</v>
+      </c>
+      <c r="I30" s="7">
+        <v>2.125</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A31" s="21" t="s">
+        <v>79</v>
+      </c>
+      <c r="B31" s="26">
+        <v>0.54545454545454541</v>
+      </c>
+      <c r="C31" s="26">
+        <v>0.45454545454545453</v>
+      </c>
+      <c r="D31" s="26">
+        <v>1</v>
+      </c>
+      <c r="H31" s="21" t="s">
+        <v>330</v>
+      </c>
+      <c r="I31" s="7">
+        <v>2.3076923076923075</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A32" s="21" t="s">
+        <v>66</v>
+      </c>
+      <c r="B32" s="26">
+        <v>0.66666666666666663</v>
+      </c>
+      <c r="C32" s="26">
+        <v>0.33333333333333331</v>
+      </c>
+      <c r="D32" s="26">
+        <v>1</v>
+      </c>
+      <c r="H32" s="21" t="s">
+        <v>333</v>
+      </c>
+      <c r="I32" s="7">
+        <v>2.2380952380952381</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A33" s="21" t="s">
+        <v>50</v>
+      </c>
+      <c r="B33" s="26">
+        <v>0.47619047619047616</v>
+      </c>
+      <c r="C33" s="26">
+        <v>0.52380952380952384</v>
+      </c>
+      <c r="D33" s="26">
+        <v>1</v>
+      </c>
+      <c r="H33" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="I33" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A34" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="B34" s="26">
+        <v>0.375</v>
+      </c>
+      <c r="C34" s="26">
+        <v>0.625</v>
+      </c>
+      <c r="D34" s="26">
+        <v>1</v>
+      </c>
+      <c r="H34" s="21" t="s">
+        <v>594</v>
+      </c>
+      <c r="I34" s="22">
+        <v>2.1818181818181817</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A35" s="21" t="s">
+        <v>26</v>
+      </c>
+      <c r="B35" s="26">
+        <v>0.61538461538461542</v>
+      </c>
+      <c r="C35" s="26">
+        <v>0.38461538461538464</v>
+      </c>
+      <c r="D35" s="26">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+      <c r="A36" s="21" t="s">
+        <v>594</v>
+      </c>
+      <c r="B36" s="26">
+        <v>0.54117647058823526</v>
+      </c>
+      <c r="C36" s="26">
+        <v>0.45882352941176469</v>
+      </c>
+      <c r="D36" s="26">
+        <v>1</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>